<commit_message>
Templates for chapter 3 and extending code capabilities
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_3.xlsx
+++ b/data/templates/dukes_ch_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8DE28-56E1-4507-A19A-5EB930258FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDD84F2-AFDC-40D7-8065-F613FB5ADE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,13 @@
     <sheet name="3.4" sheetId="4" r:id="rId4"/>
     <sheet name="3.5" sheetId="5" r:id="rId5"/>
     <sheet name="3.6" sheetId="6" r:id="rId6"/>
+    <sheet name="3.7" sheetId="7" r:id="rId7"/>
+    <sheet name="3.8" sheetId="8" r:id="rId8"/>
+    <sheet name="3.1.1" sheetId="10" r:id="rId9"/>
+    <sheet name="3.1.2" sheetId="11" r:id="rId10"/>
+    <sheet name="E.1" sheetId="12" r:id="rId11"/>
+    <sheet name="F.3" sheetId="13" r:id="rId12"/>
+    <sheet name="F.4" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="362">
   <si>
     <t>Production</t>
   </si>
@@ -567,13 +574,573 @@
   </si>
   <si>
     <t>All non-energy products</t>
+  </si>
+  <si>
+    <t>Crude oil</t>
+  </si>
+  <si>
+    <t>Natural gas liquids</t>
+  </si>
+  <si>
+    <t>Refinery feedstocks</t>
+  </si>
+  <si>
+    <t>Total primary oils</t>
+  </si>
+  <si>
+    <t>LPG</t>
+  </si>
+  <si>
+    <t>DERV</t>
+  </si>
+  <si>
+    <t>Gas oil</t>
+  </si>
+  <si>
+    <t>Fuel oil</t>
+  </si>
+  <si>
+    <t>Total petroleum products</t>
+  </si>
+  <si>
+    <t>Total oil</t>
+  </si>
+  <si>
+    <t>Primary oils</t>
+  </si>
+  <si>
+    <t>Crude oil imports</t>
+  </si>
+  <si>
+    <t>Total indigenous production</t>
+  </si>
+  <si>
+    <t>Landward indigenous production</t>
+  </si>
+  <si>
+    <t>Feedstocks indigenous production 
+[note 3]</t>
+  </si>
+  <si>
+    <t>Crude oil exports</t>
+  </si>
+  <si>
+    <t>Refinery throughput</t>
+  </si>
+  <si>
+    <t>Refinery output</t>
+  </si>
+  <si>
+    <t>Oil products exports</t>
+  </si>
+  <si>
+    <t>Oil products imports</t>
+  </si>
+  <si>
+    <t>Inland deliveries [note 4]</t>
+  </si>
+  <si>
+    <t>Crude oil 
+net exports 
+[note 5]</t>
+  </si>
+  <si>
+    <t>Oil products net exports
+[note 5]</t>
+  </si>
+  <si>
+    <t>Total net exports
+[note 5]</t>
+  </si>
+  <si>
+    <t>Ratio of crude oil imports to refinery throughput</t>
+  </si>
+  <si>
+    <t>Ratio of indigenous production to refinery throughput</t>
+  </si>
+  <si>
+    <t>Ratio of crude oil exports to indigenous production</t>
+  </si>
+  <si>
+    <t>Inland deliveries as a percentage of oil product imports
+(%)</t>
+  </si>
+  <si>
+    <t>Oil products</t>
+  </si>
+  <si>
+    <t>Inland deliveries</t>
+  </si>
+  <si>
+    <t>Feedstocks</t>
+  </si>
+  <si>
+    <t>Refinery throughout</t>
+  </si>
+  <si>
+    <t>Refiner output</t>
+  </si>
+  <si>
+    <t>Net exports</t>
+  </si>
+  <si>
+    <t>Inland deliveries as a percentage of oil product imports</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Total inland deliveries</t>
+  </si>
+  <si>
+    <t>DERV fuel</t>
+  </si>
+  <si>
+    <t>Gas oil 
+[note 3]</t>
+  </si>
+  <si>
+    <t>Fuel oils 
+[note 4]</t>
+  </si>
+  <si>
+    <t>Total deliveries for energy uses 
+[note 5]</t>
+  </si>
+  <si>
+    <t>Deliveries for non-energy uses</t>
+  </si>
+  <si>
+    <t>Electricity generator use</t>
+  </si>
+  <si>
+    <t>Gas works use</t>
+  </si>
+  <si>
+    <t>Refinery use</t>
+  </si>
+  <si>
+    <t>Other energy industry uses
+[note 6]</t>
+  </si>
+  <si>
+    <t>Iron and steel use</t>
+  </si>
+  <si>
+    <t>Other industry use</t>
+  </si>
+  <si>
+    <t>Transport use</t>
+  </si>
+  <si>
+    <t>Domestic use</t>
+  </si>
+  <si>
+    <t>Other final users
+[note 7]</t>
+  </si>
+  <si>
+    <t>Industry use</t>
+  </si>
+  <si>
+    <t>Gas flared by oil and gas terminals [note 1]</t>
+  </si>
+  <si>
+    <t>Gas flared by oil fields [note 2]</t>
+  </si>
+  <si>
+    <t>Gas flared by gas field [note 3]</t>
+  </si>
+  <si>
+    <t>Total gas flared</t>
+  </si>
+  <si>
+    <t>Gas vented by oil and gas terminals [note 1]</t>
+  </si>
+  <si>
+    <t>Gas vented by oil fields [note 2]</t>
+  </si>
+  <si>
+    <t>Gas vented by gas fields [note 3]</t>
+  </si>
+  <si>
+    <t>Total gas vented</t>
+  </si>
+  <si>
+    <t>Total gas flared and vented</t>
+  </si>
+  <si>
+    <t>Flared</t>
+  </si>
+  <si>
+    <t>Vented</t>
+  </si>
+  <si>
+    <t>Oi and gas terminals</t>
+  </si>
+  <si>
+    <t>Oil fields</t>
+  </si>
+  <si>
+    <t>Gas fields</t>
+  </si>
+  <si>
+    <t>Oil and gas terminals</t>
+  </si>
+  <si>
+    <t>Mcm</t>
+  </si>
+  <si>
+    <t>Offshore oil pipeline terminals, ethane production [note 1]</t>
+  </si>
+  <si>
+    <t>Offshore oil pipeline terminals, propane production [note 1]</t>
+  </si>
+  <si>
+    <t>Offshore oil pipeline terminals, butane production [note 1]</t>
+  </si>
+  <si>
+    <t>Offshore oil pipeline terminals, condensate production [note 1]</t>
+  </si>
+  <si>
+    <t>Total offshore oil terminal production</t>
+  </si>
+  <si>
+    <t>Offshore associated gas terminals, ethane production [note 2]</t>
+  </si>
+  <si>
+    <t>Offshore associated gas terminals, propane production [note 2]</t>
+  </si>
+  <si>
+    <t>Offshore associated gas terminals, butane production [note 2]</t>
+  </si>
+  <si>
+    <t>Offshore associated gas terminals, condensate production [note 2]</t>
+  </si>
+  <si>
+    <t>Total offshore associated gas terminal production</t>
+  </si>
+  <si>
+    <t>Offshore dry gas terminals, condensate production [note 3]</t>
+  </si>
+  <si>
+    <t>Total offshore dry gas terminal production</t>
+  </si>
+  <si>
+    <t>Onshore ethane production [note 4]</t>
+  </si>
+  <si>
+    <t>Onshore propane production [note 4]</t>
+  </si>
+  <si>
+    <t>Onshore butane production [note 4]</t>
+  </si>
+  <si>
+    <t>Onshore condensate production [note 4]</t>
+  </si>
+  <si>
+    <t>Total onshore production</t>
+  </si>
+  <si>
+    <t>Total ethane production</t>
+  </si>
+  <si>
+    <t>Total propane production</t>
+  </si>
+  <si>
+    <t>Total butane production</t>
+  </si>
+  <si>
+    <t>Total condensate production</t>
+  </si>
+  <si>
+    <t>Total production</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Onshore</t>
+  </si>
+  <si>
+    <t>Condensate</t>
+  </si>
+  <si>
+    <t>Oil terminal</t>
+  </si>
+  <si>
+    <t>Asssociatyed gas terminal</t>
+  </si>
+  <si>
+    <t>Dry gas terminal</t>
+  </si>
+  <si>
+    <t>Disposal by UK refineries</t>
+  </si>
+  <si>
+    <t>Total exports</t>
+  </si>
+  <si>
+    <t>Exports to Albania</t>
+  </si>
+  <si>
+    <t>Exports to the Bahamas [note 1]</t>
+  </si>
+  <si>
+    <t>Exports to Belgium</t>
+  </si>
+  <si>
+    <t>Exports to Brunei</t>
+  </si>
+  <si>
+    <t>Exports to Bulgaria</t>
+  </si>
+  <si>
+    <t>Exports to Canada</t>
+  </si>
+  <si>
+    <t>Exports to Chile</t>
+  </si>
+  <si>
+    <t>Exports to China</t>
+  </si>
+  <si>
+    <t>Exports to Denmark</t>
+  </si>
+  <si>
+    <t>Exports to Finland</t>
+  </si>
+  <si>
+    <t>Exports to France</t>
+  </si>
+  <si>
+    <t>Exports to Germany</t>
+  </si>
+  <si>
+    <t>Exports to Gibraltar</t>
+  </si>
+  <si>
+    <t>Exports to Greece</t>
+  </si>
+  <si>
+    <t>Exports to India</t>
+  </si>
+  <si>
+    <t>Exports to Italy</t>
+  </si>
+  <si>
+    <t>Exports to Lebanon</t>
+  </si>
+  <si>
+    <t>Exports to Lithuania</t>
+  </si>
+  <si>
+    <t>Exports to Martinique [note 1]</t>
+  </si>
+  <si>
+    <t>Exports to Morocco</t>
+  </si>
+  <si>
+    <t>Exports to the Netherlands [note 2]</t>
+  </si>
+  <si>
+    <t>Exports to Norway</t>
+  </si>
+  <si>
+    <t>Exports to Panama</t>
+  </si>
+  <si>
+    <t>Exports to Poland</t>
+  </si>
+  <si>
+    <t>Exports to Portugal</t>
+  </si>
+  <si>
+    <t>Exports to Puerto Rico</t>
+  </si>
+  <si>
+    <t>Exports to the Republic of Ireland</t>
+  </si>
+  <si>
+    <t>Exports to Singapore</t>
+  </si>
+  <si>
+    <t>Exports to South Africa</t>
+  </si>
+  <si>
+    <t>Exports to South Korea</t>
+  </si>
+  <si>
+    <t>Exports to Spain</t>
+  </si>
+  <si>
+    <t>Exports to St Lucia [note 1]</t>
+  </si>
+  <si>
+    <t>Exports to Sweden</t>
+  </si>
+  <si>
+    <t>Exports to Taiwan</t>
+  </si>
+  <si>
+    <t>Exports to Turkey</t>
+  </si>
+  <si>
+    <t>Exports to United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Exports to Uruguay</t>
+  </si>
+  <si>
+    <t>Exports to USA</t>
+  </si>
+  <si>
+    <t>Exports to Virgin Islands [note 1]</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Total disposals [note 3]</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Refinery disposals</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>St Lucia</t>
+  </si>
+  <si>
+    <t>Virgin Islands</t>
+  </si>
+  <si>
+    <t>Martinique [note</t>
+  </si>
+  <si>
+    <t>Republic</t>
+  </si>
+  <si>
+    <t>United Arab</t>
+  </si>
+  <si>
+    <t>All disposals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,16 +1155,367 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -605,19 +1523,232 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="56">
+    <cellStyle name="20% - Colore 1 2" xfId="20" xr:uid="{B82E4C63-85C2-472D-9313-1D068FE4ED5B}"/>
+    <cellStyle name="20% - Colore 2 2" xfId="24" xr:uid="{F0E8540D-2D6C-4A78-958C-9F05A92FB2F4}"/>
+    <cellStyle name="20% - Colore 3 2" xfId="28" xr:uid="{E59DC444-88D4-4A2C-AAAF-C22E0A6953C9}"/>
+    <cellStyle name="20% - Colore 4 2" xfId="32" xr:uid="{D32280A5-80DA-4B8F-BA60-B4658A5B82F8}"/>
+    <cellStyle name="20% - Colore 5 2" xfId="36" xr:uid="{39B17D9B-72E5-45D2-9E85-B2D31C0FDA2C}"/>
+    <cellStyle name="20% - Colore 6 2" xfId="40" xr:uid="{29FD2304-C42D-4B65-9E8B-7AAC7357E83A}"/>
+    <cellStyle name="40% - Colore 1 2" xfId="21" xr:uid="{29D64798-85F4-4AC0-8E3E-D96EFFF49177}"/>
+    <cellStyle name="40% - Colore 2 2" xfId="25" xr:uid="{3D54B29D-4A4E-419E-A587-3587ED2EAED6}"/>
+    <cellStyle name="40% - Colore 3 2" xfId="29" xr:uid="{DE17FA96-9186-48D8-9EC5-DE82A0EF2623}"/>
+    <cellStyle name="40% - Colore 4 2" xfId="33" xr:uid="{6AF2FE19-42B8-43A4-9814-D0F9A3A130A6}"/>
+    <cellStyle name="40% - Colore 5 2" xfId="37" xr:uid="{62ABCE71-8753-41B2-8B2C-AE81036B4A70}"/>
+    <cellStyle name="40% - Colore 6 2" xfId="41" xr:uid="{560B4198-4DF0-43DA-81CD-79B8C79FAD2F}"/>
+    <cellStyle name="60% - Colore 1 2" xfId="22" xr:uid="{601D9526-39CC-4D78-AD06-68D5F72E0BAE}"/>
+    <cellStyle name="60% - Colore 2 2" xfId="26" xr:uid="{B25E0662-471D-4092-8AA4-56DD0F886EE0}"/>
+    <cellStyle name="60% - Colore 3 2" xfId="30" xr:uid="{B6303227-810F-41D7-BA9F-FC4F99DC8189}"/>
+    <cellStyle name="60% - Colore 4 2" xfId="34" xr:uid="{D8FA09F8-F4ED-48C5-857E-92F3D0864FB1}"/>
+    <cellStyle name="60% - Colore 5 2" xfId="38" xr:uid="{E0AD42A6-2F93-4611-9E73-7C56FCE399FD}"/>
+    <cellStyle name="60% - Colore 6 2" xfId="42" xr:uid="{2CB5E3E7-DBB9-4D0D-96AE-B2E09EC41A86}"/>
+    <cellStyle name="Calcolo 2" xfId="13" xr:uid="{EF279A7B-AAF2-405E-AE4F-DB9DA1EEDC78}"/>
+    <cellStyle name="Cella collegata 2" xfId="14" xr:uid="{38DAB61D-677F-4F86-99DB-E3C74E1474DD}"/>
+    <cellStyle name="Cella da controllare 2" xfId="15" xr:uid="{B88859C7-D881-4C46-90FA-BB9A686314E4}"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="43" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="44" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Colore 1 2" xfId="19" xr:uid="{50A7E790-50A2-447D-9DE9-413A0159717F}"/>
+    <cellStyle name="Colore 2 2" xfId="23" xr:uid="{85881ABB-29F4-44C2-AD5F-73F4FF1659AB}"/>
+    <cellStyle name="Colore 3 2" xfId="27" xr:uid="{F6828A86-46B5-4D2B-937F-3BB0CCA8ED0C}"/>
+    <cellStyle name="Colore 4 2" xfId="31" xr:uid="{CF918E6C-535F-46DB-BBC4-9CFFA1C101BB}"/>
+    <cellStyle name="Colore 5 2" xfId="35" xr:uid="{047C9665-6253-46C4-ABE2-8BB0AC180F13}"/>
+    <cellStyle name="Colore 6 2" xfId="39" xr:uid="{BA11DF20-527B-401F-9E03-8BB9121416F2}"/>
+    <cellStyle name="Heading 1 2" xfId="45" xr:uid="{D12426F1-09EA-4615-AD2A-169C499444A6}"/>
+    <cellStyle name="Heading 2 2" xfId="46" xr:uid="{63BF5FB5-D519-489D-9BC7-5672539E1EC1}"/>
+    <cellStyle name="Heading 3 2" xfId="48" xr:uid="{81455525-015A-44A9-801F-FAEC54C621BB}"/>
+    <cellStyle name="Hyperlink 2" xfId="47" xr:uid="{958D4971-2F90-4DE1-B9C5-3AB93F686EE3}"/>
+    <cellStyle name="Hyperlink 3" xfId="50" xr:uid="{CC362E3F-F9F4-46A5-8E5D-EF98E13863F7}"/>
+    <cellStyle name="Input 2" xfId="11" xr:uid="{90056306-1740-4D8F-9167-A681D7ECC332}"/>
+    <cellStyle name="Neutrale 2" xfId="10" xr:uid="{06D054DC-BD24-4F43-8131-4450F1C453F9}"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{BFE09124-5B28-459A-AE78-BA451E860F3E}"/>
+    <cellStyle name="Normal 2 2" xfId="49" xr:uid="{5499EE13-8161-4240-AFBF-FEE5201666E7}"/>
+    <cellStyle name="Normal 2 3" xfId="52" xr:uid="{62C2594D-8B2D-48E5-B1D6-BF036E86DD9B}"/>
+    <cellStyle name="Normal 3" xfId="53" xr:uid="{1ABB6DCD-00F9-409B-85E8-D234B0C70A28}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{D80C3E22-1A4A-4F78-9B06-3A559D074BE6}"/>
+    <cellStyle name="Normal 4 2" xfId="55" xr:uid="{9C85CD6C-7178-461F-824E-D88DCBC337E2}"/>
+    <cellStyle name="Normal 8" xfId="54" xr:uid="{BCD94263-283E-402F-907E-7E2D8969AD7E}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale 2" xfId="2" xr:uid="{1AA33676-1828-4228-8786-379C41F3C2BD}"/>
+    <cellStyle name="Output 2" xfId="12" xr:uid="{40A1FE8C-8D9C-439B-B4B0-54CAA3BA4C31}"/>
+    <cellStyle name="Testo avviso 2" xfId="16" xr:uid="{3280F5CB-E6C7-4C5F-A7E8-6D3CEA0D7188}"/>
+    <cellStyle name="Testo descrittivo 2" xfId="17" xr:uid="{FC5968B2-6E91-41F1-99DB-72EB69AFE3D2}"/>
+    <cellStyle name="Titolo 1 2" xfId="4" xr:uid="{6B2DF65A-D8E4-4F7E-B4D9-F1ED6A62E90E}"/>
+    <cellStyle name="Titolo 2 2" xfId="5" xr:uid="{F932EB33-15EF-4EE4-94F8-DD578B84564B}"/>
+    <cellStyle name="Titolo 3 2" xfId="6" xr:uid="{0EC1F435-96CF-42D6-8A5B-E5EB4F857317}"/>
+    <cellStyle name="Titolo 4 2" xfId="7" xr:uid="{A1DF47C8-DECB-48B8-BE09-D73DA4ED785A}"/>
+    <cellStyle name="Titolo 5" xfId="3" xr:uid="{CC224EAB-F669-4B43-95F0-0EED221EDBED}"/>
+    <cellStyle name="Totale 2" xfId="18" xr:uid="{FE9E3D0D-61CA-4AE1-AA62-D16F795B3B9C}"/>
+    <cellStyle name="Valore non valido 2" xfId="9" xr:uid="{4F339B1A-382F-4C39-837F-6CD9DA842524}"/>
+    <cellStyle name="Valore valido 2" xfId="8" xr:uid="{E753F090-56F4-4C5A-8FDD-8D063A4A3E6B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1715,6 +2846,2093 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B41B7A-2C3D-4E57-995C-29C4474E4F08}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>1+A3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A20" si="0">1+A4</f>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>222</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" t="s">
+        <v>231</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F17" t="s">
+        <v>227</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" t="s">
+        <v>229</v>
+      </c>
+      <c r="F19" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0453779E-9CE9-47BE-A18A-BF56586362AF}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A11C28-B92E-4355-94B1-8B9D816B2B97}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="52.77734375" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>1+A2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A23" si="0">1+A3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" t="s">
+        <v>272</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>268</v>
+      </c>
+      <c r="C22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" t="s">
+        <v>272</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>269</v>
+      </c>
+      <c r="D23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31027A86-7F1C-468A-AAAF-6A7BB0E2B479}">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>1+A2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A44" si="0">1+A3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" t="s">
+        <v>326</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" t="s">
+        <v>328</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" t="s">
+        <v>329</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" t="s">
+        <v>331</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" t="s">
+        <v>334</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>291</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>292</v>
+      </c>
+      <c r="C18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C19" t="s">
+        <v>337</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C20" t="s">
+        <v>338</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" t="s">
+        <v>339</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>296</v>
+      </c>
+      <c r="C22" t="s">
+        <v>358</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>297</v>
+      </c>
+      <c r="C23" t="s">
+        <v>340</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>298</v>
+      </c>
+      <c r="C24" t="s">
+        <v>341</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>299</v>
+      </c>
+      <c r="C25" t="s">
+        <v>342</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>301</v>
+      </c>
+      <c r="C27" t="s">
+        <v>344</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>302</v>
+      </c>
+      <c r="C28" t="s">
+        <v>345</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" t="s">
+        <v>354</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>304</v>
+      </c>
+      <c r="C30" t="s">
+        <v>359</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>305</v>
+      </c>
+      <c r="C31" t="s">
+        <v>346</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C32" t="s">
+        <v>353</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>307</v>
+      </c>
+      <c r="C33" t="s">
+        <v>355</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>308</v>
+      </c>
+      <c r="C34" t="s">
+        <v>347</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>309</v>
+      </c>
+      <c r="C35" t="s">
+        <v>356</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C36" t="s">
+        <v>348</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>311</v>
+      </c>
+      <c r="C37" t="s">
+        <v>349</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>312</v>
+      </c>
+      <c r="C38" t="s">
+        <v>350</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>313</v>
+      </c>
+      <c r="C39" t="s">
+        <v>360</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>314</v>
+      </c>
+      <c r="C40" t="s">
+        <v>351</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>315</v>
+      </c>
+      <c r="C41" t="s">
+        <v>352</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>316</v>
+      </c>
+      <c r="C42" t="s">
+        <v>357</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>317</v>
+      </c>
+      <c r="C43" t="s">
+        <v>317</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>318</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
+        <v>361</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CC6622-CEAD-4D77-9284-6CE5F1058248}">
   <dimension ref="A1:G60"/>
@@ -3177,8 +6395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F518A5-C205-460E-8CCB-B23F7B1926B2}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3929,7 +7147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF98E2C-5059-45E8-A2AA-3D5FF548F21F}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -4513,8 +7731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D4C765-27B6-435A-8DF0-D533416DA58C}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4918,4 +8136,1192 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AF7E55-CF5E-478B-AE82-46B1BDE0FD14}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>1+A2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>1+A3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A19" si="0">1+A4</f>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52A4735-F889-4EBB-BC98-D1B3E6568DE2}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>1+A2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>1+A3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A19" si="0">1+A4</f>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467EAA01-A872-4247-975B-CBD91630A6BD}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" t="s">
+        <v>212</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" t="s">
+        <v>204</v>
+      </c>
+      <c r="G16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>205</v>
+      </c>
+      <c r="F17" t="s">
+        <v>205</v>
+      </c>
+      <c r="G17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>206</v>
+      </c>
+      <c r="F18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>